<commit_message>
fix oilPricePerLit on excel
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\korn\tech-creators\gov-logistic\govlogistic-api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F79D05-1232-48EB-868B-0BF7B59C8AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837E7C48-CF36-4317-B3FE-820DFB59AF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="4180" windowWidth="22820" windowHeight="15420" xr2:uid="{71FFFA1D-B21D-4580-A99E-09F3C483309C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71FFFA1D-B21D-4580-A99E-09F3C483309C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">                                       ตารางแสดงวงเงินงบประมาณที่ได้รับจัดสรรและราคากลาง (ราคาอ้างอิง)</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>18 ล้อ</t>
+  </si>
+  <si>
+    <t>oilPriceValue</t>
   </si>
 </sst>
 </file>
@@ -635,7 +638,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -745,8 +748,8 @@
       <c r="M5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="13">
-        <v>32</v>
+      <c r="N5" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -917,6 +920,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
@@ -933,7 +937,6 @@
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:K9"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>